<commit_message>
updating master with feature branch code
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -347,32 +347,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{ABC787E9-CCC1-4BDA-905B-4DCB5BF46B2D}" diskRevisions="1" revisionId="81" version="22">
-  <header guid="{DAAE7DA9-236E-448A-9FFF-44CBF02B5ACE}" dateTime="2019-09-10T10:04:53" maxSheetId="5" userName="admin" r:id="rId1">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{E7ADBBB7-BE90-4E94-970F-AA6A498B4FCA}" dateTime="2019-09-10T10:05:24" maxSheetId="6" userName="admin" r:id="rId2" minRId="1">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{D07CB630-2C2A-48DE-BDE3-00E9A636D595}" dateTime="2019-09-10T10:08:24" maxSheetId="6" userName="admin" r:id="rId3" minRId="2" maxRId="36">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
   <header guid="{62F86ADF-AE23-4CF3-85DA-B2FC6A622EBD}" dateTime="2019-09-10T10:10:36" maxSheetId="6" userName="admin" r:id="rId4" minRId="37" maxRId="44">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -547,10 +521,6 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rrc rId="60" sId="1" ref="A7:XFD7" action="deleteRow">
@@ -970,14 +940,6 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <ris rId="1" sheetId="5" name="[Master_Sheet.xlsx]Sheet1" sheetPosition="4"/>
-  <rcv guid="{17DC0733-3E6C-4403-A6F2-366590E0F695}" action="delete"/>
-  <rcv guid="{17DC0733-3E6C-4403-A6F2-366590E0F695}" action="add"/>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="79" sId="1">
@@ -1025,285 +987,6 @@
         <t>Y</t>
       </is>
     </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="2" sId="2">
-    <oc r="A25" t="inlineStr">
-      <is>
-        <t>3</t>
-      </is>
-    </oc>
-    <nc r="A25"/>
-  </rcc>
-  <rcc rId="3" sId="2">
-    <oc r="B25" t="inlineStr">
-      <is>
-        <t>Ganesh</t>
-      </is>
-    </oc>
-    <nc r="B25"/>
-  </rcc>
-  <rcc rId="4" sId="2">
-    <oc r="C25" t="inlineStr">
-      <is>
-        <t>Bhosale</t>
-      </is>
-    </oc>
-    <nc r="C25"/>
-  </rcc>
-  <rcc rId="5" sId="2">
-    <oc r="D25" t="inlineStr">
-      <is>
-        <t>Mumbai</t>
-      </is>
-    </oc>
-    <nc r="D25"/>
-  </rcc>
-  <rcc rId="6" sId="2">
-    <oc r="E25" t="inlineStr">
-      <is>
-        <t>9850658748</t>
-      </is>
-    </oc>
-    <nc r="E25"/>
-  </rcc>
-  <rcc rId="7" sId="2">
-    <oc r="F25" t="inlineStr">
-      <is>
-        <t>test.test1236@gmail.com</t>
-      </is>
-    </oc>
-    <nc r="F25"/>
-  </rcc>
-  <rcc rId="8" sId="2">
-    <oc r="G25" t="inlineStr">
-      <is>
-        <t>Rahul#126</t>
-      </is>
-    </oc>
-    <nc r="G25"/>
-  </rcc>
-  <rcc rId="9" sId="2">
-    <oc r="A26" t="inlineStr">
-      <is>
-        <t>4</t>
-      </is>
-    </oc>
-    <nc r="A26"/>
-  </rcc>
-  <rcc rId="10" sId="2">
-    <oc r="B26" t="inlineStr">
-      <is>
-        <t>Snehal</t>
-      </is>
-    </oc>
-    <nc r="B26"/>
-  </rcc>
-  <rcc rId="11" sId="2">
-    <oc r="C26" t="inlineStr">
-      <is>
-        <t>chopade</t>
-      </is>
-    </oc>
-    <nc r="C26"/>
-  </rcc>
-  <rcc rId="12" sId="2">
-    <oc r="D26" t="inlineStr">
-      <is>
-        <t>Delhi</t>
-      </is>
-    </oc>
-    <nc r="D26"/>
-  </rcc>
-  <rcc rId="13" sId="2">
-    <oc r="E26" t="inlineStr">
-      <is>
-        <t>2587456547</t>
-      </is>
-    </oc>
-    <nc r="E26"/>
-  </rcc>
-  <rcc rId="14" sId="2">
-    <oc r="F26" t="inlineStr">
-      <is>
-        <t>test.test1237@gmail.com</t>
-      </is>
-    </oc>
-    <nc r="F26"/>
-  </rcc>
-  <rcc rId="15" sId="2">
-    <oc r="G26" t="inlineStr">
-      <is>
-        <t>Rahul#127</t>
-      </is>
-    </oc>
-    <nc r="G26"/>
-  </rcc>
-  <rcc rId="16" sId="2">
-    <oc r="A27">
-      <v>5</v>
-    </oc>
-    <nc r="A27"/>
-  </rcc>
-  <rcc rId="17" sId="2">
-    <oc r="B27" t="inlineStr">
-      <is>
-        <t>Namita</t>
-      </is>
-    </oc>
-    <nc r="B27"/>
-  </rcc>
-  <rcc rId="18" sId="2">
-    <oc r="C27" t="inlineStr">
-      <is>
-        <t>Wikhe</t>
-      </is>
-    </oc>
-    <nc r="C27"/>
-  </rcc>
-  <rcc rId="19" sId="2">
-    <oc r="D27" t="inlineStr">
-      <is>
-        <t>USA</t>
-      </is>
-    </oc>
-    <nc r="D27"/>
-  </rcc>
-  <rcc rId="20" sId="2">
-    <oc r="E27" t="inlineStr">
-      <is>
-        <t>2587456547</t>
-      </is>
-    </oc>
-    <nc r="E27"/>
-  </rcc>
-  <rcc rId="21" sId="2">
-    <oc r="F27" t="inlineStr">
-      <is>
-        <t>test.test1235@gmail.com</t>
-      </is>
-    </oc>
-    <nc r="F27"/>
-  </rcc>
-  <rcc rId="22" sId="2">
-    <oc r="G27" t="inlineStr">
-      <is>
-        <t>Rahul#125</t>
-      </is>
-    </oc>
-    <nc r="G27"/>
-  </rcc>
-  <rcc rId="23" sId="2">
-    <oc r="A28">
-      <v>6</v>
-    </oc>
-    <nc r="A28"/>
-  </rcc>
-  <rcc rId="24" sId="2">
-    <oc r="B28" t="inlineStr">
-      <is>
-        <t>Ganesh</t>
-      </is>
-    </oc>
-    <nc r="B28"/>
-  </rcc>
-  <rcc rId="25" sId="2">
-    <oc r="C28" t="inlineStr">
-      <is>
-        <t>Bhosale</t>
-      </is>
-    </oc>
-    <nc r="C28"/>
-  </rcc>
-  <rcc rId="26" sId="2">
-    <oc r="D28" t="inlineStr">
-      <is>
-        <t>Mumbai</t>
-      </is>
-    </oc>
-    <nc r="D28"/>
-  </rcc>
-  <rcc rId="27" sId="2">
-    <oc r="E28" t="inlineStr">
-      <is>
-        <t>9850658748</t>
-      </is>
-    </oc>
-    <nc r="E28"/>
-  </rcc>
-  <rcc rId="28" sId="2">
-    <oc r="F28" t="inlineStr">
-      <is>
-        <t>test.test1236@gmail.com</t>
-      </is>
-    </oc>
-    <nc r="F28"/>
-  </rcc>
-  <rcc rId="29" sId="2">
-    <oc r="G28" t="inlineStr">
-      <is>
-        <t>Rahul#126</t>
-      </is>
-    </oc>
-    <nc r="G28"/>
-  </rcc>
-  <rcc rId="30" sId="2">
-    <oc r="A29">
-      <v>7</v>
-    </oc>
-    <nc r="A29"/>
-  </rcc>
-  <rcc rId="31" sId="2">
-    <oc r="B29" t="inlineStr">
-      <is>
-        <t>Snehal</t>
-      </is>
-    </oc>
-    <nc r="B29"/>
-  </rcc>
-  <rcc rId="32" sId="2">
-    <oc r="C29" t="inlineStr">
-      <is>
-        <t>chopade</t>
-      </is>
-    </oc>
-    <nc r="C29"/>
-  </rcc>
-  <rcc rId="33" sId="2">
-    <oc r="D29" t="inlineStr">
-      <is>
-        <t>Delhi</t>
-      </is>
-    </oc>
-    <nc r="D29"/>
-  </rcc>
-  <rcc rId="34" sId="2">
-    <oc r="E29" t="inlineStr">
-      <is>
-        <t>2587456547</t>
-      </is>
-    </oc>
-    <nc r="E29"/>
-  </rcc>
-  <rcc rId="35" sId="2">
-    <oc r="F29" t="inlineStr">
-      <is>
-        <t>test.test1237@gmail.com</t>
-      </is>
-    </oc>
-    <nc r="F29"/>
-  </rcc>
-  <rcc rId="36" sId="2">
-    <oc r="G29" t="inlineStr">
-      <is>
-        <t>Rahul#127</t>
-      </is>
-    </oc>
-    <nc r="G29"/>
   </rcc>
 </revisions>
 </file>

</xml_diff>